<commit_message>
interact process demo & misc
</commit_message>
<xml_diff>
--- a/Luban/Config/Datas/item.xlsx
+++ b/Luban/Config/Datas/item.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="69">
   <si>
     <t>##var</t>
   </si>
@@ -165,115 +165,100 @@
     <t>##comment</t>
   </si>
   <si>
-    <t>deadA</t>
-  </si>
-  <si>
-    <t>死灵卡包A</t>
+    <t>用于检查引用完整性</t>
+  </si>
+  <si>
+    <t>DIALOG/TIPS/CLOSEUP/BUBBLE/TIMELINE/GETCARDS</t>
+  </si>
+  <si>
+    <t>拉达冈的誓词</t>
+  </si>
+  <si>
+    <t>RadahNote</t>
+  </si>
+  <si>
+    <t>拉达冈的誓词，记录了黄金树的诞生</t>
+  </si>
+  <si>
+    <t>BOOK</t>
+  </si>
+  <si>
+    <t>/GameMain/Arts/Demo/UI_Icon_prop_01.png[UI_Icon_prop_01_0]</t>
+  </si>
+  <si>
+    <t>WHITE</t>
+  </si>
+  <si>
+    <t>10001,CLOSEUP,ShowCloseUp</t>
+  </si>
+  <si>
+    <t>XX卡包</t>
+  </si>
+  <si>
+    <t>Cardbag_XX</t>
+  </si>
+  <si>
+    <t>十分好用的XX卡包</t>
   </si>
   <si>
     <t>CARDBAG</t>
   </si>
   <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/64px/bow.png</t>
-  </si>
-  <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/128px/bow.png</t>
-  </si>
-  <si>
-    <t>WHITE</t>
-  </si>
-  <si>
-    <t>10000,DIALOG,GetCard</t>
-  </si>
-  <si>
-    <t>deadB</t>
-  </si>
-  <si>
-    <t>死灵卡包B</t>
-  </si>
-  <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/64px/book_open.png</t>
-  </si>
-  <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/128px/book_open.png</t>
-  </si>
-  <si>
-    <t>10001,CLOSEUP,ShowCloseUp</t>
-  </si>
-  <si>
-    <t>warriorA</t>
-  </si>
-  <si>
-    <t>战士卡包A</t>
-  </si>
-  <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/64px/award.png</t>
-  </si>
-  <si>
-    <t>/GameMain/Arts/BOARD GAME ICON/128px/award.png</t>
-  </si>
-  <si>
-    <t>wizzardA</t>
-  </si>
-  <si>
-    <t>法师卡包A</t>
-  </si>
-  <si>
-    <t>angelA</t>
-  </si>
-  <si>
-    <t>天使卡包A</t>
-  </si>
-  <si>
-    <t>pencil</t>
-  </si>
-  <si>
-    <t>把铅笔插入他的脑子</t>
-  </si>
-  <si>
-    <t>一本名叫把铅笔插入他的脑子的书</t>
-  </si>
-  <si>
-    <t>BOOK</t>
-  </si>
-  <si>
-    <t>doll</t>
-  </si>
-  <si>
-    <t>嘉琳手办</t>
+    <t>/GameMain/Arts/Demo/UI_Icon_prop_01.png[UI_Icon_prop_01_1]</t>
+  </si>
+  <si>
+    <t>10000,GETCARDS,GetCard</t>
+  </si>
+  <si>
+    <t>普通钥匙</t>
+  </si>
+  <si>
+    <t>NormalKey</t>
+  </si>
+  <si>
+    <t>普普通通平凡无奇的钥匙</t>
+  </si>
+  <si>
+    <t>KEY</t>
+  </si>
+  <si>
+    <t>/GameMain/Arts/Demo/UI_Icon_prop_01.png[UI_Icon_prop_01_2]</t>
+  </si>
+  <si>
+    <t>快乐水</t>
+  </si>
+  <si>
+    <t>HappyWater</t>
+  </si>
+  <si>
+    <t>雪崩镇生存必需品</t>
+  </si>
+  <si>
+    <t>CONSUME</t>
+  </si>
+  <si>
+    <t>/GameMain/Arts/Demo/UI_Icon_prop_01.png[UI_Icon_prop_01_3]</t>
+  </si>
+  <si>
+    <t>10000,BUBBLE,DrinkHappyWater</t>
+  </si>
+  <si>
+    <t>仙女快乐棒</t>
+  </si>
+  <si>
+    <t>HappyStick</t>
+  </si>
+  <si>
+    <t>“我从没见过这么奇怪的快乐棒”</t>
   </si>
   <si>
     <t>OTHER</t>
   </si>
   <si>
-    <t>BLUE</t>
-  </si>
-  <si>
-    <t>kitchenkit</t>
-  </si>
-  <si>
-    <t>后厨钥匙</t>
-  </si>
-  <si>
-    <t>KEY</t>
-  </si>
-  <si>
-    <t>YELLOW</t>
-  </si>
-  <si>
-    <t>chicken</t>
-  </si>
-  <si>
-    <t>疯狂星期四炸鸡</t>
-  </si>
-  <si>
-    <t>CONSUME</t>
-  </si>
-  <si>
-    <t>sause</t>
-  </si>
-  <si>
-    <t>老干爹酱料</t>
+    <t>/GameMain/Arts/Demo/UI_Icon_prop_01.png[UI_Icon_prop_01_4]</t>
+  </si>
+  <si>
+    <t>10000,DIALOG,CheckHappyStick</t>
   </si>
 </sst>
 </file>
@@ -281,9 +266,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
@@ -309,6 +294,120 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="等线"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -317,51 +416,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -369,75 +423,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="等线"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="等线"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -466,19 +451,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -496,19 +553,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -520,43 +589,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -568,43 +601,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -616,25 +613,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,32 +648,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -704,17 +663,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -737,8 +690,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -747,16 +700,48 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -766,10 +751,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -778,137 +763,137 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="31" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="7" applyAlignment="1"/>
@@ -927,6 +912,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1249,8 +1237,10 @@
   <sheetPr/>
   <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection/>
+      <selection pane="topRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.95" customHeight="1"/>
@@ -1259,13 +1249,13 @@
     <col min="2" max="2" width="13.75" customWidth="1"/>
     <col min="3" max="3" width="11.625" customWidth="1"/>
     <col min="4" max="4" width="25" customWidth="1"/>
-    <col min="5" max="5" width="28.875" customWidth="1"/>
+    <col min="5" max="5" width="35.125" customWidth="1"/>
     <col min="6" max="6" width="19.625" customWidth="1"/>
     <col min="7" max="7" width="8.25" customWidth="1"/>
     <col min="8" max="8" width="15.375" customWidth="1"/>
     <col min="9" max="9" width="25.875" customWidth="1"/>
-    <col min="10" max="10" width="51.25" customWidth="1"/>
-    <col min="11" max="11" width="51.625" customWidth="1"/>
+    <col min="10" max="10" width="55.875" customWidth="1"/>
+    <col min="11" max="11" width="55.125" customWidth="1"/>
     <col min="12" max="12" width="21.5" customWidth="1"/>
     <col min="13" max="13" width="29.375" customWidth="1"/>
     <col min="14" max="14" width="66.25" customWidth="1"/>
@@ -1519,33 +1509,40 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="I5" s="7" t="s">
+        <v>37</v>
+      </c>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
       <c r="M5" s="7"/>
-      <c r="N5" s="11"/>
+      <c r="N5" s="11" t="s">
+        <v>38</v>
+      </c>
       <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
+      <c r="P5" s="13"/>
     </row>
-    <row r="6" customHeight="1" spans="2:16">
+    <row r="6" customHeight="1" spans="1:15">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
       <c r="B6">
         <v>10000</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E6" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="G6">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1554,38 +1551,40 @@
         <v>10001</v>
       </c>
       <c r="J6" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="L6" t="b">
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>42</v>
-      </c>
-      <c r="N6" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
+      </c>
+      <c r="N6" s="13" t="s">
+        <v>45</v>
       </c>
       <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
     </row>
-    <row r="7" customHeight="1" spans="2:14">
+    <row r="7" customHeight="1" spans="1:16">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
       <c r="B7">
         <v>10001</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="E7" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="F7" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="G7">
         <v>100</v>
@@ -1597,39 +1596,44 @@
         <v>10002</v>
       </c>
       <c r="J7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="K7" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L7" t="b">
         <v>1</v>
       </c>
       <c r="M7" t="s">
-        <v>42</v>
-      </c>
-      <c r="N7" s="12" t="s">
-        <v>48</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="O7" s="12"/>
+      <c r="P7" s="13"/>
     </row>
-    <row r="8" customHeight="1" spans="2:13">
+    <row r="8" customHeight="1" spans="1:15">
+      <c r="A8" t="s">
+        <v>52</v>
+      </c>
       <c r="B8">
         <v>10002</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E8" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>55</v>
       </c>
       <c r="G8">
-        <v>60</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -1638,283 +1642,111 @@
         <v>10003</v>
       </c>
       <c r="J8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K8" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="L8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M8" t="s">
-        <v>42</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="O8" s="12"/>
     </row>
-    <row r="9" customHeight="1" spans="2:13">
+    <row r="9" customHeight="1" spans="1:15">
+      <c r="A9" t="s">
+        <v>57</v>
+      </c>
       <c r="B9">
         <v>10003</v>
       </c>
       <c r="C9" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="D9" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="G9">
-        <v>60</v>
+        <v>10</v>
       </c>
       <c r="H9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <v>10004</v>
       </c>
       <c r="J9" t="s">
-        <v>40</v>
+        <v>61</v>
       </c>
       <c r="K9" t="s">
-        <v>41</v>
+        <v>61</v>
       </c>
       <c r="L9" t="b">
         <v>1</v>
       </c>
       <c r="M9" t="s">
-        <v>42</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="O9" s="12"/>
     </row>
-    <row r="10" customHeight="1" spans="2:13">
+    <row r="10" customHeight="1" spans="1:15">
+      <c r="A10" t="s">
+        <v>63</v>
+      </c>
       <c r="B10">
         <v>10004</v>
       </c>
       <c r="C10" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="D10" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="E10" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="F10" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="G10">
-        <v>60</v>
+        <v>300</v>
       </c>
       <c r="H10">
         <v>1</v>
       </c>
       <c r="I10">
-        <v>10005</v>
+        <v>10004</v>
       </c>
       <c r="J10" t="s">
-        <v>40</v>
+        <v>67</v>
       </c>
       <c r="K10" t="s">
-        <v>41</v>
+        <v>67</v>
       </c>
       <c r="L10" t="b">
         <v>1</v>
       </c>
       <c r="M10" t="s">
-        <v>42</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O10" s="12"/>
     </row>
-    <row r="11" customHeight="1" spans="2:13">
-      <c r="B11">
-        <v>10005</v>
-      </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11" t="s">
-        <v>58</v>
-      </c>
-      <c r="E11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F11" t="s">
-        <v>60</v>
-      </c>
-      <c r="G11">
-        <v>180</v>
-      </c>
-      <c r="H11">
-        <v>1</v>
-      </c>
-      <c r="I11">
-        <v>10006</v>
-      </c>
-      <c r="J11" t="s">
-        <v>40</v>
-      </c>
-      <c r="K11" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" t="b">
-        <v>1</v>
-      </c>
-      <c r="M11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" customHeight="1" spans="2:13">
-      <c r="B12">
-        <v>10006</v>
-      </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" t="s">
-        <v>62</v>
-      </c>
-      <c r="E12" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12">
-        <v>1000</v>
-      </c>
-      <c r="H12">
-        <v>1</v>
-      </c>
-      <c r="I12">
-        <v>10007</v>
-      </c>
-      <c r="J12" t="s">
-        <v>40</v>
-      </c>
-      <c r="K12" t="s">
-        <v>41</v>
-      </c>
-      <c r="L12" t="b">
-        <v>1</v>
-      </c>
-      <c r="M12" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" customHeight="1" spans="2:13">
-      <c r="B13">
-        <v>10007</v>
-      </c>
-      <c r="C13" t="s">
-        <v>65</v>
-      </c>
-      <c r="D13" t="s">
-        <v>66</v>
-      </c>
-      <c r="E13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" t="s">
-        <v>67</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-      <c r="I13">
-        <v>10008</v>
-      </c>
-      <c r="J13" t="s">
-        <v>40</v>
-      </c>
-      <c r="K13" t="s">
-        <v>41</v>
-      </c>
-      <c r="L13" t="b">
-        <v>0</v>
-      </c>
-      <c r="M13" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" customHeight="1" spans="2:13">
-      <c r="B14">
-        <v>10008</v>
-      </c>
-      <c r="C14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E14" t="s">
-        <v>70</v>
-      </c>
-      <c r="F14" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G14">
-        <v>30</v>
-      </c>
-      <c r="H14">
-        <v>5</v>
-      </c>
-      <c r="I14">
-        <v>10009</v>
-      </c>
-      <c r="J14" t="s">
-        <v>40</v>
-      </c>
-      <c r="K14" t="s">
-        <v>41</v>
-      </c>
-      <c r="L14" t="b">
-        <v>1</v>
-      </c>
-      <c r="M14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="15" customHeight="1" spans="2:13">
-      <c r="B15">
-        <v>10009</v>
-      </c>
-      <c r="C15" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" t="s">
-        <v>73</v>
-      </c>
-      <c r="E15" t="s">
-        <v>73</v>
-      </c>
-      <c r="F15" s="8" t="s">
-        <v>71</v>
-      </c>
-      <c r="G15">
-        <v>5</v>
-      </c>
-      <c r="H15">
-        <v>5</v>
-      </c>
-      <c r="I15">
-        <v>10000</v>
-      </c>
-      <c r="J15" t="s">
-        <v>40</v>
-      </c>
-      <c r="K15" t="s">
-        <v>41</v>
-      </c>
-      <c r="L15" t="b">
-        <v>1</v>
-      </c>
-      <c r="M15" t="s">
-        <v>68</v>
-      </c>
+    <row r="15" customHeight="1" spans="6:6">
+      <c r="F15" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>